<commit_message>
added populations to prioritization
</commit_message>
<xml_diff>
--- a/docs/Snake River IPTDS Prioritization 20230606.xlsx
+++ b/docs/Snake River IPTDS Prioritization 20230606.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeR_IPTDS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92629D75-AF50-4CF1-8886-8ACB1A1D3784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B526AB-E2CC-4CF1-88B1-4ED099B805E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-2385" windowWidth="25800" windowHeight="21150" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-2385" windowWidth="25800" windowHeight="21150" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -19,11 +19,6 @@
     <sheet name="STHD_Prioritization" sheetId="6" r:id="rId4"/>
     <sheet name="prev_comanager_iptds" sheetId="4" r:id="rId5"/>
   </sheets>
-  <definedNames>
-    <definedName name="node_count">#REF!</definedName>
-    <definedName name="pops">#REF!</definedName>
-    <definedName name="ryan">prev_comanager_iptds!$A$1:$Y$88</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -277,7 +272,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3334" uniqueCount="777">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3783" uniqueCount="857">
   <si>
     <t>site</t>
   </si>
@@ -2626,10 +2621,250 @@
     <t>AH</t>
   </si>
   <si>
-    <t>mpg</t>
-  </si>
-  <si>
-    <t>trt_popid</t>
+    <t>MPG</t>
+  </si>
+  <si>
+    <t>Monitoring Type</t>
+  </si>
+  <si>
+    <t>Population Determination (Figure 1)</t>
+  </si>
+  <si>
+    <t>Upgrade</t>
+  </si>
+  <si>
+    <t>Budget/Responsibility</t>
+  </si>
+  <si>
+    <t>ESU_DPS</t>
+  </si>
+  <si>
+    <t>Snake River Spring/Summer-run Chinook Salmon ESU</t>
+  </si>
+  <si>
+    <t>Lookingglass Creek</t>
+  </si>
+  <si>
+    <t>GRLOO</t>
+  </si>
+  <si>
+    <t>Camas Creek</t>
+  </si>
+  <si>
+    <t>MFCAM</t>
+  </si>
+  <si>
+    <t>Chamberlain Creek</t>
+  </si>
+  <si>
+    <t>SRCHA</t>
+  </si>
+  <si>
+    <t>Loon Creek</t>
+  </si>
+  <si>
+    <t>MFLOO</t>
+  </si>
+  <si>
+    <t>Middle Fork Salmon River above Indian Creek</t>
+  </si>
+  <si>
+    <t>MFUMA</t>
+  </si>
+  <si>
+    <t>Middle Fork Salmon River below Indian Creek</t>
+  </si>
+  <si>
+    <t>MFLMA</t>
+  </si>
+  <si>
+    <t>Sulphur Creek</t>
+  </si>
+  <si>
+    <t>MFSUL</t>
+  </si>
+  <si>
+    <t>East Fork Salmon River</t>
+  </si>
+  <si>
+    <t>SREFS</t>
+  </si>
+  <si>
+    <t>SRPAH</t>
+  </si>
+  <si>
+    <t>Lower North Fork Clearwater</t>
+  </si>
+  <si>
+    <t>NCLMA</t>
+  </si>
+  <si>
+    <t>Meadow Creek</t>
+  </si>
+  <si>
+    <t>SEMEA</t>
+  </si>
+  <si>
+    <t>Moose Creek</t>
+  </si>
+  <si>
+    <t>SEMOO</t>
+  </si>
+  <si>
+    <t>Upper North Fork Clearwater</t>
+  </si>
+  <si>
+    <t>NCUMA</t>
+  </si>
+  <si>
+    <t>Upper Selway River</t>
+  </si>
+  <si>
+    <t>SEUMA</t>
+  </si>
+  <si>
+    <t>POP_NAME</t>
+  </si>
+  <si>
+    <t>Snake River Basin Steelhead DPS</t>
+  </si>
+  <si>
+    <t>Hells Canyon</t>
+  </si>
+  <si>
+    <t>CRNFC-s</t>
+  </si>
+  <si>
+    <t>SNHCT-s</t>
+  </si>
+  <si>
+    <t>SRCHA-s</t>
+  </si>
+  <si>
+    <t>SREFS-s</t>
+  </si>
+  <si>
+    <t>North Fork Clearwater River</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Extirpated</t>
+  </si>
+  <si>
+    <t>Functionally Extirpated</t>
+  </si>
+  <si>
+    <t>Unlisted</t>
+  </si>
+  <si>
+    <t>Extant</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Data Gap</t>
+  </si>
+  <si>
+    <t>Upgrade?</t>
+  </si>
+  <si>
+    <t>Budget/Responsibility?</t>
+  </si>
+  <si>
+    <t>Do not include in Biomark</t>
+  </si>
+  <si>
+    <t>high precision is not necessary b/c of TUC, and weir operation gives us another low precision method (doesn't cover all MaSAs) so IPTDS is redundant</t>
+  </si>
+  <si>
+    <t>Include in Biomark</t>
+  </si>
+  <si>
+    <t>Potlatch-consider upgrade; Lapwai - LAP; Big Canyon - Data Gap; Lawyer Creek - Data Gap; Lower SFCLW Tribs - Data Gap</t>
+  </si>
+  <si>
+    <t>LRL, LRU</t>
+  </si>
+  <si>
+    <t>LC1, LC2</t>
+  </si>
+  <si>
+    <t>Consider upgrading LC1</t>
+  </si>
+  <si>
+    <t>SW1, SW2</t>
+  </si>
+  <si>
+    <t>SC1, SC2</t>
+  </si>
+  <si>
+    <t>Could support SC3, SC4 instead with CRA as back-up</t>
+  </si>
+  <si>
+    <t>Wenaha - WEN; Mud Creek - Data Gap</t>
+  </si>
+  <si>
+    <t>UGR, (UGS or CCU)</t>
+  </si>
+  <si>
+    <t>Consider upgrading URG</t>
+  </si>
+  <si>
+    <t>WR1, MR1, WR2</t>
+  </si>
+  <si>
+    <t>Consider upgrading WR1</t>
+  </si>
+  <si>
+    <t>IR1, IR2</t>
+  </si>
+  <si>
+    <t>Consider upgrading IR1</t>
+  </si>
+  <si>
+    <t>Canidate/increase and include in Biomark O&amp;M</t>
+  </si>
+  <si>
+    <t>Little Salmon - Data Gap</t>
+  </si>
+  <si>
+    <t>SFG, (KRS or EFSF)</t>
+  </si>
+  <si>
+    <t>TAY, Camas - Data Gap, Loon - Data Gap</t>
+  </si>
+  <si>
+    <t>Marsh Creek - MAR; Marble, Pistol, Rapid, Upper Middle, Bear Valley are Data Gaps</t>
+  </si>
+  <si>
+    <t>Split between MFSR pops is below Loon Creek</t>
+  </si>
+  <si>
+    <t>USE, USI</t>
+  </si>
+  <si>
+    <t>Consider upgrading/moving</t>
+  </si>
+  <si>
+    <t>Challis and EFSR - Data Gap</t>
+  </si>
+  <si>
+    <t>Consider upgrading</t>
+  </si>
+  <si>
+    <t>YFK VC2, Upper Salmon, Basin, Thompson - Data Gap</t>
+  </si>
+  <si>
+    <t>IPTDS w/in Steelhead MaSA (Figure 2)</t>
+  </si>
+  <si>
+    <t>IPTDS w/in Chinook MaSA (Figure 2)</t>
   </si>
 </sst>
 </file>
@@ -3289,8 +3524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A42020D-9532-4D3F-8F80-EE8C6D0895CA}">
   <dimension ref="B1:AA67"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4060,11 +4295,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4554933-5C62-409C-B1F4-87485B7250BD}">
   <dimension ref="A1:AH101"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4105,11 +4340,11 @@
     <col min="34" max="34" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="33" t="s">
         <v>215</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="33" t="s">
         <v>216</v>
       </c>
       <c r="C1" s="35" t="s">
@@ -4205,7 +4440,7 @@
       <c r="AG1" s="35" t="s">
         <v>625</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AH1" s="33" t="s">
         <v>221</v>
       </c>
     </row>
@@ -13685,20 +13920,791 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{055B48E5-B2D0-4B19-967E-72BE4D4B4F25}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="46.7265625" style="33" customWidth="1"/>
+    <col min="2" max="2" width="22.90625" style="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" style="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.1796875" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.81640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>780</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>775</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="6" t="s">
+        <v>521</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>809</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>817</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>776</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>777</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>856</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>778</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>779</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>797</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>796</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>753</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>613</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>752</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>798</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>756</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>751</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>616</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>754</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>755</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>761</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>762</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>760</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>186</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>757</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>758</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>745</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>748</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>612</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>745</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>746</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>745</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>785</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>784</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>745</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>787</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>786</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>745</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>789</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>788</v>
+      </c>
+      <c r="E15" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>745</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>750</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B17" s="33" t="s">
+        <v>745</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>791</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>790</v>
+      </c>
+      <c r="E17" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>745</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>793</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>792</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>745</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>795</v>
+      </c>
+      <c r="D19" s="33" t="s">
+        <v>794</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>744</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>738</v>
+      </c>
+      <c r="D21" s="33" t="s">
+        <v>739</v>
+      </c>
+      <c r="E21" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B22" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>743</v>
+      </c>
+      <c r="D22" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B23" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>741</v>
+      </c>
+      <c r="D23" s="33" t="s">
+        <v>742</v>
+      </c>
+      <c r="E23" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B24" s="33" t="s">
+        <v>729</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>765</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>729</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>736</v>
+      </c>
+      <c r="D25" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="E25" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B26" s="33" t="s">
+        <v>729</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>737</v>
+      </c>
+      <c r="D26" s="33" t="s">
+        <v>735</v>
+      </c>
+      <c r="E26" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B27" s="33" t="s">
+        <v>729</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>763</v>
+      </c>
+      <c r="D27" s="33" t="s">
+        <v>764</v>
+      </c>
+      <c r="E27" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B28" s="33" t="s">
+        <v>729</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>783</v>
+      </c>
+      <c r="D28" s="33" t="s">
+        <v>782</v>
+      </c>
+      <c r="E28" s="33" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>729</v>
+      </c>
+      <c r="C29" s="33" t="s">
+        <v>732</v>
+      </c>
+      <c r="D29" s="33" t="s">
+        <v>733</v>
+      </c>
+      <c r="E29" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B30" s="33" t="s">
+        <v>729</v>
+      </c>
+      <c r="C30" s="33" t="s">
+        <v>734</v>
+      </c>
+      <c r="D30" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="E30" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B31" s="33" t="s">
+        <v>729</v>
+      </c>
+      <c r="C31" s="33" t="s">
+        <v>730</v>
+      </c>
+      <c r="D31" s="33" t="s">
+        <v>146</v>
+      </c>
+      <c r="E31" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B32" s="33" t="s">
+        <v>713</v>
+      </c>
+      <c r="C32" s="33" t="s">
+        <v>728</v>
+      </c>
+      <c r="D32" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="E32" s="33" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B33" s="33" t="s">
+        <v>713</v>
+      </c>
+      <c r="C33" s="33" t="s">
+        <v>714</v>
+      </c>
+      <c r="D33" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="E33" s="33" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B34" s="33" t="s">
+        <v>715</v>
+      </c>
+      <c r="C34" s="33" t="s">
+        <v>716</v>
+      </c>
+      <c r="D34" s="33" t="s">
+        <v>717</v>
+      </c>
+      <c r="E34" s="33" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B35" s="33" t="s">
+        <v>715</v>
+      </c>
+      <c r="C35" s="33" t="s">
+        <v>724</v>
+      </c>
+      <c r="D35" s="33" t="s">
+        <v>611</v>
+      </c>
+      <c r="E35" s="33" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B36" s="33" t="s">
+        <v>715</v>
+      </c>
+      <c r="C36" s="33" t="s">
+        <v>720</v>
+      </c>
+      <c r="D36" s="33" t="s">
+        <v>721</v>
+      </c>
+      <c r="E36" s="33" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B37" s="33" t="s">
+        <v>715</v>
+      </c>
+      <c r="C37" s="33" t="s">
+        <v>726</v>
+      </c>
+      <c r="D37" s="33" t="s">
+        <v>727</v>
+      </c>
+      <c r="E37" s="33" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B38" s="33" t="s">
+        <v>722</v>
+      </c>
+      <c r="C38" s="33" t="s">
+        <v>725</v>
+      </c>
+      <c r="D38" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="E38" s="33" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B39" s="33" t="s">
+        <v>722</v>
+      </c>
+      <c r="C39" s="33" t="s">
+        <v>723</v>
+      </c>
+      <c r="D39" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="E39" s="33" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B40" s="33" t="s">
+        <v>722</v>
+      </c>
+      <c r="C40" s="33" t="s">
+        <v>800</v>
+      </c>
+      <c r="D40" s="33" t="s">
+        <v>799</v>
+      </c>
+      <c r="E40" s="33" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B41" s="33" t="s">
+        <v>722</v>
+      </c>
+      <c r="C41" s="33" t="s">
+        <v>802</v>
+      </c>
+      <c r="D41" s="33" t="s">
+        <v>801</v>
+      </c>
+      <c r="E41" s="33" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B42" s="33" t="s">
+        <v>722</v>
+      </c>
+      <c r="C42" s="33" t="s">
+        <v>804</v>
+      </c>
+      <c r="D42" s="33" t="s">
+        <v>803</v>
+      </c>
+      <c r="E42" s="33" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B43" s="33" t="s">
+        <v>722</v>
+      </c>
+      <c r="C43" s="33" t="s">
+        <v>806</v>
+      </c>
+      <c r="D43" s="33" t="s">
+        <v>805</v>
+      </c>
+      <c r="E43" s="33" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" s="33" t="s">
+        <v>781</v>
+      </c>
+      <c r="B44" s="33" t="s">
+        <v>722</v>
+      </c>
+      <c r="C44" s="33" t="s">
+        <v>808</v>
+      </c>
+      <c r="D44" s="33" t="s">
+        <v>807</v>
+      </c>
+      <c r="E44" s="33" t="s">
+        <v>820</v>
       </c>
     </row>
   </sheetData>
@@ -13708,15 +14714,759 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{175A1EF7-D6F6-40B5-8CC5-720EBF0869DB}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="2" max="2" width="18" style="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.26953125" style="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.26953125" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6328125" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.08984375" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.81640625" style="33" customWidth="1"/>
+    <col min="8" max="8" width="32" customWidth="1"/>
+    <col min="9" max="9" width="9.08984375" style="33" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.08984375" style="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="129.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>780</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>775</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>521</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>809</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>817</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>776</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>777</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>855</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>825</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>826</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>810</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>620</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>747</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>821</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>823</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>844</v>
+      </c>
+      <c r="H2" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>810</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>620</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>814</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>786</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>821</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>824</v>
+      </c>
+      <c r="G3" s="33" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>810</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>620</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>815</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>796</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>821</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>824</v>
+      </c>
+      <c r="G4" s="33" t="s">
+        <v>844</v>
+      </c>
+      <c r="H4" t="s">
+        <v>852</v>
+      </c>
+      <c r="K4" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>810</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>620</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>205</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>613</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>821</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>822</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>829</v>
+      </c>
+      <c r="H5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>810</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>620</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>206</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>740</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>821</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>824</v>
+      </c>
+      <c r="G6" s="33" t="s">
+        <v>844</v>
+      </c>
+      <c r="H6" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>810</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>620</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>749</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>821</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>823</v>
+      </c>
+      <c r="G7" s="33" t="s">
+        <v>844</v>
+      </c>
+      <c r="H7" t="s">
+        <v>848</v>
+      </c>
+      <c r="K7" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>810</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>620</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>207</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>821</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>822</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>829</v>
+      </c>
+      <c r="H8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>810</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>620</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>756</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>821</v>
+      </c>
+      <c r="F9" s="33" t="s">
+        <v>822</v>
+      </c>
+      <c r="G9" s="33" t="s">
+        <v>829</v>
+      </c>
+      <c r="H9" t="s">
+        <v>850</v>
+      </c>
+      <c r="K9" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>810</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>620</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>616</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>821</v>
+      </c>
+      <c r="F10" s="33" t="s">
+        <v>822</v>
+      </c>
+      <c r="G10" s="33" t="s">
+        <v>829</v>
+      </c>
+      <c r="H10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>810</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>620</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>210</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>759</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>821</v>
+      </c>
+      <c r="F11" s="33" t="s">
+        <v>822</v>
+      </c>
+      <c r="G11" s="33" t="s">
+        <v>829</v>
+      </c>
+      <c r="H11" t="s">
+        <v>854</v>
+      </c>
+      <c r="K11" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>810</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>620</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>202</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>821</v>
+      </c>
+      <c r="F12" s="33" t="s">
+        <v>822</v>
+      </c>
+      <c r="G12" s="33" t="s">
+        <v>829</v>
+      </c>
+      <c r="H12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>810</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>620</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>821</v>
+      </c>
+      <c r="F13" s="33" t="s">
+        <v>822</v>
+      </c>
+      <c r="G13" s="33" t="s">
+        <v>829</v>
+      </c>
+      <c r="H13" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>810</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>718</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>719</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>821</v>
+      </c>
+      <c r="F14" s="33" t="s">
+        <v>823</v>
+      </c>
+      <c r="G14" s="33" t="s">
+        <v>829</v>
+      </c>
+      <c r="H14" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>810</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>718</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="E15" s="33" t="s">
+        <v>821</v>
+      </c>
+      <c r="F15" s="33" t="s">
+        <v>822</v>
+      </c>
+      <c r="G15" s="33" t="s">
+        <v>829</v>
+      </c>
+      <c r="H15" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>810</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>718</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>191</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>821</v>
+      </c>
+      <c r="F16" s="33" t="s">
+        <v>822</v>
+      </c>
+      <c r="G16" s="33" t="s">
+        <v>829</v>
+      </c>
+      <c r="H16" t="s">
+        <v>832</v>
+      </c>
+      <c r="K16" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>810</v>
+      </c>
+      <c r="B17" s="33" t="s">
+        <v>718</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>812</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>816</v>
+      </c>
+      <c r="E17" s="33" t="s">
+        <v>818</v>
+      </c>
+      <c r="F17" s="33" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>810</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>718</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>821</v>
+      </c>
+      <c r="F18" s="33" t="s">
+        <v>822</v>
+      </c>
+      <c r="G18" s="33" t="s">
+        <v>829</v>
+      </c>
+      <c r="H18" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>810</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>718</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="D19" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>821</v>
+      </c>
+      <c r="F19" s="33" t="s">
+        <v>822</v>
+      </c>
+      <c r="G19" s="33" t="s">
+        <v>829</v>
+      </c>
+      <c r="H19" t="s">
+        <v>835</v>
+      </c>
+      <c r="K19" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>810</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>731</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>821</v>
+      </c>
+      <c r="F20" s="33" t="s">
+        <v>823</v>
+      </c>
+      <c r="G20" s="33" t="s">
+        <v>829</v>
+      </c>
+      <c r="H20" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>810</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="D21" s="33" t="s">
+        <v>735</v>
+      </c>
+      <c r="E21" s="33" t="s">
+        <v>821</v>
+      </c>
+      <c r="F21" s="33" t="s">
+        <v>822</v>
+      </c>
+      <c r="G21" s="33" t="s">
+        <v>829</v>
+      </c>
+      <c r="H21" t="s">
+        <v>838</v>
+      </c>
+      <c r="K21" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>810</v>
+      </c>
+      <c r="B22" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="D22" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>821</v>
+      </c>
+      <c r="F22" s="33" t="s">
+        <v>822</v>
+      </c>
+      <c r="G22" s="33" t="s">
+        <v>829</v>
+      </c>
+      <c r="H22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>810</v>
+      </c>
+      <c r="B23" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="D23" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="E23" s="33" t="s">
+        <v>821</v>
+      </c>
+      <c r="F23" s="33" t="s">
+        <v>822</v>
+      </c>
+      <c r="G23" s="33" t="s">
+        <v>829</v>
+      </c>
+      <c r="H23" t="s">
+        <v>840</v>
+      </c>
+      <c r="K23" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>810</v>
+      </c>
+      <c r="B24" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>821</v>
+      </c>
+      <c r="F24" s="33" t="s">
+        <v>822</v>
+      </c>
+      <c r="G24" s="33" t="s">
+        <v>829</v>
+      </c>
+      <c r="H24" t="s">
+        <v>842</v>
+      </c>
+      <c r="K24" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>810</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>811</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>813</v>
+      </c>
+      <c r="D25" s="33" t="s">
+        <v>811</v>
+      </c>
+      <c r="E25" s="33" t="s">
+        <v>818</v>
+      </c>
+      <c r="F25" s="33" t="s">
+        <v>822</v>
+      </c>
+      <c r="G25" s="33" t="s">
+        <v>844</v>
+      </c>
+      <c r="H25" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>810</v>
+      </c>
+      <c r="B26" s="33" t="s">
+        <v>713</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>203</v>
+      </c>
+      <c r="D26" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="E26" s="33" t="s">
+        <v>821</v>
+      </c>
+      <c r="F26" s="33" t="s">
+        <v>822</v>
+      </c>
+      <c r="G26" s="33" t="s">
+        <v>827</v>
+      </c>
+      <c r="K26" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>810</v>
+      </c>
+      <c r="B27" s="33" t="s">
+        <v>713</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>204</v>
+      </c>
+      <c r="D27" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="E27" s="33" t="s">
+        <v>821</v>
+      </c>
+      <c r="F27" s="33" t="s">
+        <v>822</v>
+      </c>
+      <c r="G27" s="33" t="s">
+        <v>829</v>
+      </c>
+      <c r="H27" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added sr traps and weirs from ptagis
</commit_message>
<xml_diff>
--- a/docs/Snake River IPTDS Prioritization 20230606.xlsx
+++ b/docs/Snake River IPTDS Prioritization 20230606.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeR_IPTDS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685183C5-B124-4235-BEA5-D74CBA0FC053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE867E92-5D30-4701-A585-2DEC981CC56E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54600" yWindow="-2385" windowWidth="25800" windowHeight="21150" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="54600" yWindow="-2385" windowWidth="25800" windowHeight="21150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="prev_comanager_iptds" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3531,8 +3530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A42020D-9532-4D3F-8F80-EE8C6D0895CA}">
   <dimension ref="B1:AA67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4302,7 +4301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4554933-5C62-409C-B1F4-87485B7250BD}">
   <dimension ref="A1:AH101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
added antenna counts to site prioritization
</commit_message>
<xml_diff>
--- a/docs/Snake River IPTDS Prioritization 20230606.xlsx
+++ b/docs/Snake River IPTDS Prioritization 20230606.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeR_IPTDS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C2C853-6FC1-45D5-A98B-15FEFF0F61D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E3034A-88D8-4FDD-96A6-1A522C94A52F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2505" windowWidth="51840" windowHeight="21390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-2385" windowWidth="25800" windowHeight="21150" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -524,7 +524,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4371" uniqueCount="898">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4372" uniqueCount="900">
   <si>
     <t>site</t>
   </si>
@@ -3262,6 +3262,12 @@
   </si>
   <si>
     <t>Fund NFS</t>
+  </si>
+  <si>
+    <t>ptagis_active</t>
+  </si>
+  <si>
+    <t>antenna_count</t>
   </si>
 </sst>
 </file>
@@ -4800,54 +4806,55 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4554933-5C62-409C-B1F4-87485B7250BD}">
-  <dimension ref="A1:AH101"/>
+  <dimension ref="A1:AI101"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomRight" activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.08984375" style="33" customWidth="1"/>
-    <col min="2" max="2" width="28.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" style="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7265625" style="33" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.6328125" style="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.6328125" style="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.08984375" style="33" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" style="33" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.453125" style="33" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.90625" style="33" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21" style="33" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="44.1796875" style="33" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.90625" style="33" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18" style="33" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.6328125" style="33" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="42.26953125" style="33" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.6328125" style="33" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.81640625" style="33" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.08984375" style="33" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.90625" style="34" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.6328125" style="34" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18" style="33" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20.1796875" style="33" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.90625" style="33" customWidth="1"/>
-    <col min="24" max="24" width="18" style="33" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="26.453125" style="33" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.7265625" style="33" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11" style="33" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.7265625" style="33" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="24.36328125" style="33" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.7265625" style="33" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="25.08984375" style="33" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="23.26953125" style="33" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="21.26953125" style="33" customWidth="1"/>
-    <col min="34" max="34" width="16" customWidth="1"/>
+    <col min="5" max="5" width="33.36328125" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.54296875" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.36328125" style="33" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.08984375" style="33" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.36328125" style="33" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.08984375" style="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="49.1796875" style="33" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.6328125" style="33" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.90625" style="33" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15" style="33" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="47" style="33" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.36328125" style="33" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.6328125" style="33" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.08984375" style="33" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.54296875" style="34" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15" style="34" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.90625" style="33" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.08984375" style="33" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.54296875" style="33" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.90625" style="33" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="28.453125" style="33" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.6328125" style="33" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.08984375" style="33" customWidth="1"/>
+    <col min="28" max="28" width="15.26953125" style="33" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.54296875" style="33" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="26.54296875" style="33" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.36328125" style="33" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="27.26953125" style="33" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="25.453125" style="33" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="30.6328125" style="33" customWidth="1"/>
+    <col min="35" max="35" width="15.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="33" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="33" t="s">
         <v>214</v>
       </c>
@@ -4924,34 +4931,37 @@
         <v>621</v>
       </c>
       <c r="Z1" s="35" t="s">
-        <v>535</v>
+        <v>898</v>
       </c>
       <c r="AA1" s="33" t="s">
         <v>521</v>
       </c>
-      <c r="AB1" s="35" t="s">
+      <c r="AB1" s="33" t="s">
+        <v>899</v>
+      </c>
+      <c r="AC1" s="35" t="s">
         <v>536</v>
       </c>
-      <c r="AC1" s="35" t="s">
+      <c r="AD1" s="35" t="s">
         <v>525</v>
       </c>
-      <c r="AD1" s="35" t="s">
+      <c r="AE1" s="35" t="s">
         <v>526</v>
       </c>
-      <c r="AE1" s="35" t="s">
+      <c r="AF1" s="35" t="s">
         <v>527</v>
       </c>
-      <c r="AF1" s="35" t="s">
+      <c r="AG1" s="35" t="s">
         <v>627</v>
       </c>
-      <c r="AG1" s="35" t="s">
+      <c r="AH1" s="35" t="s">
         <v>624</v>
       </c>
-      <c r="AH1" s="33" t="s">
+      <c r="AI1" s="33" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="33" t="s">
         <v>96</v>
       </c>
@@ -5030,23 +5040,26 @@
       <c r="AA2" s="33">
         <v>3</v>
       </c>
-      <c r="AB2" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC2" s="36" t="s">
+      <c r="AB2" s="33">
+        <v>25</v>
+      </c>
+      <c r="AC2" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD2" s="36" t="s">
+      <c r="AE2" s="36" t="s">
         <v>562</v>
       </c>
-      <c r="AE2" s="36"/>
       <c r="AF2" s="36"/>
-      <c r="AG2" s="37"/>
-      <c r="AH2" t="s">
+      <c r="AG2" s="36"/>
+      <c r="AH2" s="37"/>
+      <c r="AI2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="33" t="s">
         <v>97</v>
       </c>
@@ -5125,23 +5138,26 @@
       <c r="AA3" s="33">
         <v>2</v>
       </c>
-      <c r="AB3" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC3" s="36" t="s">
+      <c r="AB3" s="33">
+        <v>12</v>
+      </c>
+      <c r="AC3" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="36" t="s">
         <v>549</v>
       </c>
-      <c r="AD3" s="36" t="s">
+      <c r="AE3" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE3" s="36"/>
       <c r="AF3" s="36"/>
-      <c r="AG3" s="37"/>
-      <c r="AH3" t="s">
+      <c r="AG3" s="36"/>
+      <c r="AH3" s="37"/>
+      <c r="AI3" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="33" t="s">
         <v>98</v>
       </c>
@@ -5220,23 +5236,26 @@
       <c r="AA4" s="33">
         <v>2</v>
       </c>
-      <c r="AB4" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC4" s="36" t="s">
+      <c r="AB4" s="33">
+        <v>6</v>
+      </c>
+      <c r="AC4" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD4" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD4" s="36" t="s">
+      <c r="AE4" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE4" s="36"/>
       <c r="AF4" s="36"/>
-      <c r="AG4" s="37"/>
-      <c r="AH4" t="s">
+      <c r="AG4" s="36"/>
+      <c r="AH4" s="37"/>
+      <c r="AI4" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="33" t="s">
         <v>99</v>
       </c>
@@ -5315,21 +5334,24 @@
       <c r="AA5" s="33">
         <v>3</v>
       </c>
-      <c r="AB5" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC5" s="36"/>
-      <c r="AD5" s="36" t="s">
+      <c r="AB5" s="33">
+        <v>18</v>
+      </c>
+      <c r="AC5" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="36"/>
+      <c r="AE5" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE5" s="36"/>
       <c r="AF5" s="36"/>
-      <c r="AG5" s="37"/>
-      <c r="AH5" t="s">
+      <c r="AG5" s="36"/>
+      <c r="AH5" s="37"/>
+      <c r="AI5" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="33" t="s">
         <v>100</v>
       </c>
@@ -5408,23 +5430,26 @@
       <c r="AA6" s="33">
         <v>2</v>
       </c>
-      <c r="AB6" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC6" s="36" t="s">
+      <c r="AB6" s="33">
+        <v>5</v>
+      </c>
+      <c r="AC6" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD6" s="36" t="s">
+      <c r="AE6" s="36" t="s">
         <v>554</v>
       </c>
-      <c r="AE6" s="36"/>
       <c r="AF6" s="36"/>
-      <c r="AG6" s="37"/>
-      <c r="AH6" t="s">
+      <c r="AG6" s="36"/>
+      <c r="AH6" s="37"/>
+      <c r="AI6" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" s="33" t="s">
         <v>239</v>
       </c>
@@ -5495,19 +5520,22 @@
       <c r="AA7" s="33">
         <v>2</v>
       </c>
-      <c r="AB7" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC7" s="36"/>
+      <c r="AB7" s="33">
+        <v>2</v>
+      </c>
+      <c r="AC7" s="34" t="b">
+        <v>1</v>
+      </c>
       <c r="AD7" s="36"/>
       <c r="AE7" s="36"/>
       <c r="AF7" s="36"/>
-      <c r="AG7" s="37"/>
-      <c r="AH7" t="s">
+      <c r="AG7" s="36"/>
+      <c r="AH7" s="37"/>
+      <c r="AI7" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A8" s="33" t="s">
         <v>42</v>
       </c>
@@ -5586,23 +5614,26 @@
       <c r="AA8" s="33">
         <v>3</v>
       </c>
-      <c r="AB8" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC8" s="36" t="s">
+      <c r="AB8" s="33">
+        <v>10</v>
+      </c>
+      <c r="AC8" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD8" s="36" t="s">
+      <c r="AE8" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE8" s="36"/>
       <c r="AF8" s="36"/>
-      <c r="AG8" s="37"/>
-      <c r="AH8" t="s">
+      <c r="AG8" s="36"/>
+      <c r="AH8" s="37"/>
+      <c r="AI8" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A9" s="33" t="s">
         <v>43</v>
       </c>
@@ -5681,23 +5712,26 @@
       <c r="AA9" s="33">
         <v>3</v>
       </c>
-      <c r="AB9" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC9" s="36" t="s">
+      <c r="AB9" s="33">
+        <v>3</v>
+      </c>
+      <c r="AC9" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD9" s="36" t="s">
         <v>549</v>
       </c>
-      <c r="AD9" s="36" t="s">
+      <c r="AE9" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE9" s="36"/>
       <c r="AF9" s="36"/>
-      <c r="AG9" s="37"/>
-      <c r="AH9" t="s">
+      <c r="AG9" s="36"/>
+      <c r="AH9" s="37"/>
+      <c r="AI9" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A10" s="33" t="s">
         <v>45</v>
       </c>
@@ -5776,23 +5810,26 @@
       <c r="AA10" s="33">
         <v>2</v>
       </c>
-      <c r="AB10" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC10" s="36" t="s">
+      <c r="AB10" s="33">
+        <v>2</v>
+      </c>
+      <c r="AC10" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD10" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD10" s="36" t="s">
+      <c r="AE10" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE10" s="36"/>
       <c r="AF10" s="36"/>
-      <c r="AG10" s="37"/>
-      <c r="AH10" t="s">
+      <c r="AG10" s="36"/>
+      <c r="AH10" s="37"/>
+      <c r="AI10" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A11" s="33" t="s">
         <v>44</v>
       </c>
@@ -5871,23 +5908,26 @@
       <c r="AA11" s="33">
         <v>2</v>
       </c>
-      <c r="AB11" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC11" s="36" t="s">
+      <c r="AB11" s="33">
+        <v>2</v>
+      </c>
+      <c r="AC11" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD11" s="36" t="s">
         <v>549</v>
       </c>
-      <c r="AD11" s="36" t="s">
+      <c r="AE11" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE11" s="36"/>
       <c r="AF11" s="36"/>
-      <c r="AG11" s="37"/>
-      <c r="AH11" t="s">
+      <c r="AG11" s="36"/>
+      <c r="AH11" s="37"/>
+      <c r="AI11" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A12" s="33" t="s">
         <v>46</v>
       </c>
@@ -5966,25 +6006,28 @@
       <c r="AA12" s="33">
         <v>1</v>
       </c>
-      <c r="AB12" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC12" s="36" t="s">
+      <c r="AB12" s="33">
+        <v>14</v>
+      </c>
+      <c r="AC12" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD12" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD12" s="36" t="s">
+      <c r="AE12" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE12" s="36"/>
       <c r="AF12" s="36"/>
-      <c r="AG12" s="37" t="s">
+      <c r="AG12" s="36"/>
+      <c r="AH12" s="37" t="s">
         <v>553</v>
       </c>
-      <c r="AH12" t="s">
+      <c r="AI12" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A13" s="33" t="s">
         <v>47</v>
       </c>
@@ -6063,23 +6106,26 @@
       <c r="AA13" s="33">
         <v>2</v>
       </c>
-      <c r="AB13" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC13" s="36" t="s">
+      <c r="AB13" s="33">
+        <v>14</v>
+      </c>
+      <c r="AC13" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD13" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD13" s="36" t="s">
+      <c r="AE13" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE13" s="36"/>
       <c r="AF13" s="36"/>
-      <c r="AG13" s="37"/>
-      <c r="AH13" t="s">
+      <c r="AG13" s="36"/>
+      <c r="AH13" s="37"/>
+      <c r="AI13" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A14" s="33" t="s">
         <v>48</v>
       </c>
@@ -6158,27 +6204,30 @@
       <c r="AA14" s="33">
         <v>2</v>
       </c>
-      <c r="AB14" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC14" s="36" t="s">
+      <c r="AB14" s="33">
+        <v>2</v>
+      </c>
+      <c r="AC14" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD14" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD14" s="36" t="s">
+      <c r="AE14" s="36" t="s">
         <v>554</v>
       </c>
-      <c r="AE14" s="36" t="s">
+      <c r="AF14" s="36" t="s">
         <v>555</v>
       </c>
-      <c r="AF14" s="36"/>
-      <c r="AG14" s="37" t="s">
+      <c r="AG14" s="36"/>
+      <c r="AH14" s="37" t="s">
         <v>557</v>
       </c>
-      <c r="AH14" t="s">
+      <c r="AI14" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A15" s="33" t="s">
         <v>49</v>
       </c>
@@ -6257,25 +6306,28 @@
       <c r="AA15" s="33">
         <v>2</v>
       </c>
-      <c r="AB15" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC15" s="36" t="s">
+      <c r="AB15" s="33">
+        <v>4</v>
+      </c>
+      <c r="AC15" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD15" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD15" s="36" t="s">
+      <c r="AE15" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE15" s="36" t="s">
+      <c r="AF15" s="36" t="s">
         <v>555</v>
       </c>
-      <c r="AF15" s="36"/>
-      <c r="AG15" s="37"/>
-      <c r="AH15" t="s">
+      <c r="AG15" s="36"/>
+      <c r="AH15" s="37"/>
+      <c r="AI15" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A16" s="33" t="s">
         <v>51</v>
       </c>
@@ -6354,25 +6406,28 @@
       <c r="AA16" s="33">
         <v>2</v>
       </c>
-      <c r="AB16" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC16" s="36" t="s">
+      <c r="AB16" s="33">
+        <v>2</v>
+      </c>
+      <c r="AC16" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD16" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD16" s="36" t="s">
+      <c r="AE16" s="36" t="s">
         <v>554</v>
       </c>
-      <c r="AE16" s="36" t="s">
+      <c r="AF16" s="36" t="s">
         <v>555</v>
       </c>
-      <c r="AF16" s="36"/>
-      <c r="AG16" s="37"/>
-      <c r="AH16" t="s">
+      <c r="AG16" s="36"/>
+      <c r="AH16" s="37"/>
+      <c r="AI16" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A17" s="33" t="s">
         <v>50</v>
       </c>
@@ -6451,23 +6506,26 @@
       <c r="AA17" s="33">
         <v>2</v>
       </c>
-      <c r="AB17" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC17" s="36" t="s">
+      <c r="AB17" s="33">
+        <v>6</v>
+      </c>
+      <c r="AC17" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD17" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD17" s="36" t="s">
+      <c r="AE17" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE17" s="36"/>
       <c r="AF17" s="36"/>
-      <c r="AG17" s="37"/>
-      <c r="AH17" t="s">
+      <c r="AG17" s="36"/>
+      <c r="AH17" s="37"/>
+      <c r="AI17" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A18" s="33" t="s">
         <v>52</v>
       </c>
@@ -6546,23 +6604,26 @@
       <c r="AA18" s="33">
         <v>2</v>
       </c>
-      <c r="AB18" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC18" s="36" t="s">
+      <c r="AB18" s="33">
+        <v>2</v>
+      </c>
+      <c r="AC18" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD18" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD18" s="36" t="s">
+      <c r="AE18" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE18" s="36"/>
       <c r="AF18" s="36"/>
-      <c r="AG18" s="37"/>
-      <c r="AH18" t="s">
+      <c r="AG18" s="36"/>
+      <c r="AH18" s="37"/>
+      <c r="AI18" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A19" s="33" t="s">
         <v>56</v>
       </c>
@@ -6641,25 +6702,28 @@
       <c r="AA19" s="33">
         <v>1</v>
       </c>
-      <c r="AB19" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC19" s="36" t="s">
+      <c r="AB19" s="33">
+        <v>4</v>
+      </c>
+      <c r="AC19" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD19" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD19" s="36" t="s">
+      <c r="AE19" s="36" t="s">
         <v>562</v>
       </c>
-      <c r="AE19" s="36"/>
       <c r="AF19" s="36"/>
-      <c r="AG19" s="37" t="s">
+      <c r="AG19" s="36"/>
+      <c r="AH19" s="37" t="s">
         <v>567</v>
       </c>
-      <c r="AH19" t="s">
+      <c r="AI19" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A20" s="33" t="s">
         <v>57</v>
       </c>
@@ -6738,25 +6802,28 @@
       <c r="AA20" s="33">
         <v>1</v>
       </c>
-      <c r="AB20" s="34" t="b">
+      <c r="AB20" s="33">
+        <v>4</v>
+      </c>
+      <c r="AC20" s="34" t="b">
         <v>0</v>
       </c>
-      <c r="AC20" s="36" t="s">
+      <c r="AD20" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD20" s="36" t="s">
+      <c r="AE20" s="36" t="s">
         <v>562</v>
       </c>
-      <c r="AE20" s="36"/>
       <c r="AF20" s="36"/>
-      <c r="AG20" s="37" t="s">
+      <c r="AG20" s="36"/>
+      <c r="AH20" s="37" t="s">
         <v>568</v>
       </c>
-      <c r="AH20" t="s">
+      <c r="AI20" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A21" s="33" t="s">
         <v>280</v>
       </c>
@@ -6827,19 +6894,22 @@
       <c r="AA21" s="33">
         <v>2</v>
       </c>
-      <c r="AB21" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC21" s="36"/>
+      <c r="AB21" s="33">
+        <v>2</v>
+      </c>
+      <c r="AC21" s="34" t="b">
+        <v>1</v>
+      </c>
       <c r="AD21" s="36"/>
       <c r="AE21" s="36"/>
       <c r="AF21" s="36"/>
-      <c r="AG21" s="37"/>
-      <c r="AH21" t="s">
+      <c r="AG21" s="36"/>
+      <c r="AH21" s="37"/>
+      <c r="AI21" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A22" s="33" t="s">
         <v>284</v>
       </c>
@@ -6910,19 +6980,22 @@
       <c r="AA22" s="33">
         <v>2</v>
       </c>
-      <c r="AB22" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC22" s="36"/>
+      <c r="AB22" s="33">
+        <v>4</v>
+      </c>
+      <c r="AC22" s="34" t="b">
+        <v>1</v>
+      </c>
       <c r="AD22" s="36"/>
       <c r="AE22" s="36"/>
       <c r="AF22" s="36"/>
-      <c r="AG22" s="37"/>
-      <c r="AH22" t="s">
+      <c r="AG22" s="36"/>
+      <c r="AH22" s="37"/>
+      <c r="AI22" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A23" s="33" t="s">
         <v>60</v>
       </c>
@@ -7001,25 +7074,28 @@
       <c r="AA23" s="33">
         <v>1</v>
       </c>
-      <c r="AB23" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC23" s="36" t="s">
+      <c r="AB23" s="33">
+        <v>7</v>
+      </c>
+      <c r="AC23" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD23" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD23" s="36" t="s">
+      <c r="AE23" s="36" t="s">
         <v>562</v>
       </c>
-      <c r="AE23" s="36"/>
       <c r="AF23" s="36"/>
-      <c r="AG23" s="37" t="s">
+      <c r="AG23" s="36"/>
+      <c r="AH23" s="37" t="s">
         <v>572</v>
       </c>
-      <c r="AH23" t="s">
+      <c r="AI23" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A24" s="33" t="s">
         <v>61</v>
       </c>
@@ -7098,25 +7174,28 @@
       <c r="AA24" s="33">
         <v>1</v>
       </c>
-      <c r="AB24" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC24" s="36" t="s">
+      <c r="AB24" s="33">
+        <v>6</v>
+      </c>
+      <c r="AC24" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD24" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD24" s="36" t="s">
+      <c r="AE24" s="36" t="s">
         <v>562</v>
       </c>
-      <c r="AE24" s="36"/>
       <c r="AF24" s="36"/>
-      <c r="AG24" s="37" t="s">
+      <c r="AG24" s="36"/>
+      <c r="AH24" s="37" t="s">
         <v>573</v>
       </c>
-      <c r="AH24" t="s">
+      <c r="AI24" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A25" s="33" t="s">
         <v>53</v>
       </c>
@@ -7195,23 +7274,26 @@
       <c r="AA25" s="33">
         <v>1</v>
       </c>
-      <c r="AB25" s="34" t="b">
+      <c r="AB25" s="33">
+        <v>5</v>
+      </c>
+      <c r="AC25" s="34" t="b">
         <v>0</v>
       </c>
-      <c r="AC25" s="36" t="s">
+      <c r="AD25" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD25" s="36" t="s">
+      <c r="AE25" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE25" s="36"/>
       <c r="AF25" s="36"/>
-      <c r="AG25" s="37"/>
-      <c r="AH25" t="s">
+      <c r="AG25" s="36"/>
+      <c r="AH25" s="37"/>
+      <c r="AI25" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A26" s="33" t="s">
         <v>54</v>
       </c>
@@ -7290,25 +7372,28 @@
       <c r="AA26" s="33">
         <v>1</v>
       </c>
-      <c r="AB26" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC26" s="36" t="s">
+      <c r="AB26" s="33">
+        <v>13</v>
+      </c>
+      <c r="AC26" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD26" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD26" s="36" t="s">
+      <c r="AE26" s="36" t="s">
         <v>562</v>
       </c>
-      <c r="AE26" s="36"/>
       <c r="AF26" s="36"/>
-      <c r="AG26" s="37" t="s">
+      <c r="AG26" s="36"/>
+      <c r="AH26" s="37" t="s">
         <v>565</v>
       </c>
-      <c r="AH26" t="s">
+      <c r="AI26" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A27" s="33" t="s">
         <v>55</v>
       </c>
@@ -7387,25 +7472,28 @@
       <c r="AA27" s="33">
         <v>1</v>
       </c>
-      <c r="AB27" s="34" t="b">
+      <c r="AB27" s="33">
+        <v>18</v>
+      </c>
+      <c r="AC27" s="34" t="b">
         <v>0</v>
       </c>
-      <c r="AC27" s="36" t="s">
+      <c r="AD27" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD27" s="36" t="s">
+      <c r="AE27" s="36" t="s">
         <v>562</v>
       </c>
-      <c r="AE27" s="36"/>
       <c r="AF27" s="36"/>
-      <c r="AG27" s="37" t="s">
+      <c r="AG27" s="36"/>
+      <c r="AH27" s="37" t="s">
         <v>566</v>
       </c>
-      <c r="AH27" t="s">
+      <c r="AI27" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A28" s="33" t="s">
         <v>58</v>
       </c>
@@ -7484,25 +7572,28 @@
       <c r="AA28" s="33">
         <v>1</v>
       </c>
-      <c r="AB28" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC28" s="36" t="s">
+      <c r="AB28" s="33">
+        <v>19</v>
+      </c>
+      <c r="AC28" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD28" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD28" s="36" t="s">
+      <c r="AE28" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE28" s="36"/>
       <c r="AF28" s="36"/>
-      <c r="AG28" s="37" t="s">
+      <c r="AG28" s="36"/>
+      <c r="AH28" s="37" t="s">
         <v>570</v>
       </c>
-      <c r="AH28" t="s">
+      <c r="AI28" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A29" s="33" t="s">
         <v>59</v>
       </c>
@@ -7581,25 +7672,28 @@
       <c r="AA29" s="33">
         <v>1</v>
       </c>
-      <c r="AB29" s="34" t="b">
+      <c r="AB29" s="33">
+        <v>18</v>
+      </c>
+      <c r="AC29" s="34" t="b">
         <v>0</v>
       </c>
-      <c r="AC29" s="36" t="s">
+      <c r="AD29" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD29" s="36" t="s">
+      <c r="AE29" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE29" s="36"/>
       <c r="AF29" s="36"/>
-      <c r="AG29" s="37" t="s">
+      <c r="AG29" s="36"/>
+      <c r="AH29" s="37" t="s">
         <v>571</v>
       </c>
-      <c r="AH29" t="s">
+      <c r="AI29" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A30" s="33" t="s">
         <v>62</v>
       </c>
@@ -7678,25 +7772,28 @@
       <c r="AA30" s="33">
         <v>1</v>
       </c>
-      <c r="AB30" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC30" s="36" t="s">
+      <c r="AB30" s="33">
+        <v>5</v>
+      </c>
+      <c r="AC30" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD30" s="36" t="s">
         <v>549</v>
       </c>
-      <c r="AD30" s="36" t="s">
+      <c r="AE30" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE30" s="36" t="s">
+      <c r="AF30" s="36" t="s">
         <v>574</v>
       </c>
-      <c r="AF30" s="36"/>
-      <c r="AG30" s="37"/>
-      <c r="AH30" t="s">
+      <c r="AG30" s="36"/>
+      <c r="AH30" s="37"/>
+      <c r="AI30" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A31" s="33" t="s">
         <v>63</v>
       </c>
@@ -7775,25 +7872,28 @@
       <c r="AA31" s="33">
         <v>2</v>
       </c>
-      <c r="AB31" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC31" s="36" t="s">
+      <c r="AB31" s="33">
+        <v>9</v>
+      </c>
+      <c r="AC31" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD31" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD31" s="36" t="s">
+      <c r="AE31" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE31" s="36" t="s">
+      <c r="AF31" s="36" t="s">
         <v>574</v>
       </c>
-      <c r="AF31" s="36"/>
-      <c r="AG31" s="37"/>
-      <c r="AH31" t="s">
+      <c r="AG31" s="36"/>
+      <c r="AH31" s="37"/>
+      <c r="AI31" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A32" s="33" t="s">
         <v>64</v>
       </c>
@@ -7872,25 +7972,28 @@
       <c r="AA32" s="33">
         <v>2</v>
       </c>
-      <c r="AB32" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC32" s="36" t="s">
+      <c r="AB32" s="33">
+        <v>4</v>
+      </c>
+      <c r="AC32" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD32" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD32" s="36" t="s">
+      <c r="AE32" s="36" t="s">
         <v>554</v>
       </c>
-      <c r="AE32" s="36" t="s">
+      <c r="AF32" s="36" t="s">
         <v>575</v>
       </c>
-      <c r="AF32" s="36"/>
-      <c r="AG32" s="37"/>
-      <c r="AH32" t="s">
+      <c r="AG32" s="36"/>
+      <c r="AH32" s="37"/>
+      <c r="AI32" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A33" s="33" t="s">
         <v>92</v>
       </c>
@@ -7969,25 +8072,28 @@
       <c r="AA33" s="33">
         <v>3</v>
       </c>
-      <c r="AB33" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC33" s="36" t="s">
+      <c r="AB33" s="33">
+        <v>10</v>
+      </c>
+      <c r="AC33" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD33" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD33" s="36" t="s">
+      <c r="AE33" s="36" t="s">
         <v>562</v>
       </c>
-      <c r="AE33" s="36" t="s">
+      <c r="AF33" s="36" t="s">
         <v>592</v>
       </c>
-      <c r="AF33" s="36"/>
-      <c r="AG33" s="37"/>
-      <c r="AH33" t="s">
+      <c r="AG33" s="36"/>
+      <c r="AH33" s="37"/>
+      <c r="AI33" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A34" s="33" t="s">
         <v>93</v>
       </c>
@@ -8066,25 +8172,28 @@
       <c r="AA34" s="33">
         <v>2</v>
       </c>
-      <c r="AB34" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC34" s="36" t="s">
+      <c r="AB34" s="33">
+        <v>5</v>
+      </c>
+      <c r="AC34" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD34" s="36" t="s">
         <v>549</v>
       </c>
-      <c r="AD34" s="36" t="s">
+      <c r="AE34" s="36" t="s">
         <v>554</v>
       </c>
-      <c r="AE34" s="36" t="s">
+      <c r="AF34" s="36" t="s">
         <v>592</v>
       </c>
-      <c r="AF34" s="36"/>
-      <c r="AG34" s="37"/>
-      <c r="AH34" t="s">
+      <c r="AG34" s="36"/>
+      <c r="AH34" s="37"/>
+      <c r="AI34" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A35" s="33" t="s">
         <v>94</v>
       </c>
@@ -8163,25 +8272,28 @@
       <c r="AA35" s="33">
         <v>3</v>
       </c>
-      <c r="AB35" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC35" s="36" t="s">
+      <c r="AB35" s="33">
+        <v>7</v>
+      </c>
+      <c r="AC35" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD35" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD35" s="36" t="s">
+      <c r="AE35" s="36" t="s">
         <v>554</v>
       </c>
-      <c r="AE35" s="36" t="s">
+      <c r="AF35" s="36" t="s">
         <v>592</v>
       </c>
-      <c r="AF35" s="36"/>
-      <c r="AG35" s="37"/>
-      <c r="AH35" t="s">
+      <c r="AG35" s="36"/>
+      <c r="AH35" s="37"/>
+      <c r="AI35" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A36" s="33" t="s">
         <v>95</v>
       </c>
@@ -8260,25 +8372,28 @@
       <c r="AA36" s="33">
         <v>3</v>
       </c>
-      <c r="AB36" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC36" s="36" t="s">
+      <c r="AB36" s="33">
+        <v>6</v>
+      </c>
+      <c r="AC36" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD36" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD36" s="36" t="s">
+      <c r="AE36" s="36" t="s">
         <v>554</v>
       </c>
-      <c r="AE36" s="36" t="s">
+      <c r="AF36" s="36" t="s">
         <v>592</v>
       </c>
-      <c r="AF36" s="36"/>
-      <c r="AG36" s="37"/>
-      <c r="AH36" t="s">
+      <c r="AG36" s="36"/>
+      <c r="AH36" s="37"/>
+      <c r="AI36" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A37" s="33" t="s">
         <v>65</v>
       </c>
@@ -8357,23 +8472,26 @@
       <c r="AA37" s="33">
         <v>2</v>
       </c>
-      <c r="AB37" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC37" s="36" t="s">
+      <c r="AB37" s="33">
+        <v>10</v>
+      </c>
+      <c r="AC37" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD37" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD37" s="36" t="s">
+      <c r="AE37" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE37" s="36"/>
       <c r="AF37" s="36"/>
-      <c r="AG37" s="37"/>
-      <c r="AH37" t="s">
+      <c r="AG37" s="36"/>
+      <c r="AH37" s="37"/>
+      <c r="AI37" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A38" s="33" t="s">
         <v>66</v>
       </c>
@@ -8452,25 +8570,28 @@
       <c r="AA38" s="33">
         <v>2</v>
       </c>
-      <c r="AB38" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC38" s="36" t="s">
+      <c r="AB38" s="33">
+        <v>9</v>
+      </c>
+      <c r="AC38" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD38" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD38" s="36" t="s">
+      <c r="AE38" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE38" s="36"/>
-      <c r="AF38" s="36" t="s">
+      <c r="AF38" s="36"/>
+      <c r="AG38" s="36" t="s">
         <v>577</v>
       </c>
-      <c r="AG38" s="37"/>
-      <c r="AH38" t="s">
+      <c r="AH38" s="37"/>
+      <c r="AI38" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A39" s="33" t="s">
         <v>71</v>
       </c>
@@ -8549,27 +8670,30 @@
       <c r="AA39" s="33">
         <v>1</v>
       </c>
-      <c r="AB39" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC39" s="36" t="s">
+      <c r="AB39" s="33">
+        <v>6</v>
+      </c>
+      <c r="AC39" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD39" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD39" s="36" t="s">
+      <c r="AE39" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="AE39" s="36"/>
-      <c r="AF39" s="36" t="s">
+      <c r="AF39" s="36"/>
+      <c r="AG39" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="AG39" s="37" t="s">
+      <c r="AH39" s="37" t="s">
         <v>584</v>
       </c>
-      <c r="AH39" t="s">
+      <c r="AI39" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A40" s="33" t="s">
         <v>72</v>
       </c>
@@ -8648,27 +8772,30 @@
       <c r="AA40" s="33">
         <v>2</v>
       </c>
-      <c r="AB40" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC40" s="36" t="s">
+      <c r="AB40" s="33">
+        <v>10</v>
+      </c>
+      <c r="AC40" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD40" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD40" s="36" t="s">
+      <c r="AE40" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="AE40" s="36"/>
-      <c r="AF40" s="36" t="s">
+      <c r="AF40" s="36"/>
+      <c r="AG40" s="36" t="s">
         <v>577</v>
       </c>
-      <c r="AG40" s="37" t="s">
+      <c r="AH40" s="37" t="s">
         <v>585</v>
       </c>
-      <c r="AH40" t="s">
+      <c r="AI40" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A41" s="33" t="s">
         <v>73</v>
       </c>
@@ -8747,27 +8874,30 @@
       <c r="AA41" s="33">
         <v>2</v>
       </c>
-      <c r="AB41" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC41" s="36" t="s">
+      <c r="AB41" s="33">
+        <v>8</v>
+      </c>
+      <c r="AC41" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD41" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD41" s="36" t="s">
+      <c r="AE41" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="AE41" s="36"/>
-      <c r="AF41" s="36" t="s">
+      <c r="AF41" s="36"/>
+      <c r="AG41" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="AG41" s="37" t="s">
+      <c r="AH41" s="37" t="s">
         <v>586</v>
       </c>
-      <c r="AH41" t="s">
+      <c r="AI41" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A42" s="33" t="s">
         <v>67</v>
       </c>
@@ -8846,27 +8976,30 @@
       <c r="AA42" s="33">
         <v>1</v>
       </c>
-      <c r="AB42" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC42" s="36" t="s">
+      <c r="AB42" s="33">
+        <v>6</v>
+      </c>
+      <c r="AC42" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD42" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD42" s="36" t="s">
+      <c r="AE42" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="AE42" s="36"/>
-      <c r="AF42" s="36" t="s">
+      <c r="AF42" s="36"/>
+      <c r="AG42" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="AG42" s="37" t="s">
+      <c r="AH42" s="37" t="s">
         <v>580</v>
       </c>
-      <c r="AH42" t="s">
+      <c r="AI42" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A43" s="33" t="s">
         <v>69</v>
       </c>
@@ -8945,25 +9078,28 @@
       <c r="AA43" s="33">
         <v>2</v>
       </c>
-      <c r="AB43" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC43" s="36" t="s">
+      <c r="AB43" s="33">
+        <v>4</v>
+      </c>
+      <c r="AC43" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD43" s="36" t="s">
         <v>549</v>
       </c>
-      <c r="AD43" s="36" t="s">
+      <c r="AE43" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE43" s="36"/>
-      <c r="AF43" s="36" t="s">
+      <c r="AF43" s="36"/>
+      <c r="AG43" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="AG43" s="37"/>
-      <c r="AH43" t="s">
+      <c r="AH43" s="37"/>
+      <c r="AI43" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A44" s="33" t="s">
         <v>68</v>
       </c>
@@ -9042,27 +9178,30 @@
       <c r="AA44" s="33">
         <v>2</v>
       </c>
-      <c r="AB44" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC44" s="36" t="s">
+      <c r="AB44" s="33">
+        <v>4</v>
+      </c>
+      <c r="AC44" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD44" s="36" t="s">
         <v>549</v>
       </c>
-      <c r="AD44" s="36" t="s">
+      <c r="AE44" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="AE44" s="36"/>
-      <c r="AF44" s="36" t="s">
+      <c r="AF44" s="36"/>
+      <c r="AG44" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="AG44" s="37" t="s">
+      <c r="AH44" s="37" t="s">
         <v>581</v>
       </c>
-      <c r="AH44" t="s">
+      <c r="AI44" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A45" s="33" t="s">
         <v>70</v>
       </c>
@@ -9141,27 +9280,30 @@
       <c r="AA45" s="33">
         <v>3</v>
       </c>
-      <c r="AB45" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC45" s="36" t="s">
+      <c r="AB45" s="33">
+        <v>16</v>
+      </c>
+      <c r="AC45" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD45" s="36" t="s">
         <v>549</v>
       </c>
-      <c r="AD45" s="36" t="s">
+      <c r="AE45" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="AE45" s="36"/>
-      <c r="AF45" s="36" t="s">
+      <c r="AF45" s="36"/>
+      <c r="AG45" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="AG45" s="37" t="s">
+      <c r="AH45" s="37" t="s">
         <v>583</v>
       </c>
-      <c r="AH45" t="s">
+      <c r="AI45" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A46" s="33" t="s">
         <v>120</v>
       </c>
@@ -9240,23 +9382,26 @@
       <c r="AA46" s="33">
         <v>2</v>
       </c>
-      <c r="AB46" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC46" s="36" t="s">
+      <c r="AB46" s="33">
+        <v>4</v>
+      </c>
+      <c r="AC46" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD46" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD46" s="36" t="s">
+      <c r="AE46" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE46" s="36"/>
       <c r="AF46" s="36"/>
-      <c r="AG46" s="37"/>
-      <c r="AH46" t="s">
+      <c r="AG46" s="36"/>
+      <c r="AH46" s="37"/>
+      <c r="AI46" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A47" s="33" t="s">
         <v>87</v>
       </c>
@@ -9335,23 +9480,26 @@
       <c r="AA47" s="33">
         <v>1</v>
       </c>
-      <c r="AB47" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC47" s="36" t="s">
+      <c r="AB47" s="33">
+        <v>6</v>
+      </c>
+      <c r="AC47" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD47" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD47" s="36" t="s">
+      <c r="AE47" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE47" s="36"/>
       <c r="AF47" s="36"/>
-      <c r="AG47" s="37"/>
-      <c r="AH47" t="s">
+      <c r="AG47" s="36"/>
+      <c r="AH47" s="37"/>
+      <c r="AI47" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A48" s="33" t="s">
         <v>91</v>
       </c>
@@ -9430,23 +9578,26 @@
       <c r="AA48" s="33">
         <v>2</v>
       </c>
-      <c r="AB48" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC48" s="36" t="s">
+      <c r="AB48" s="33">
+        <v>10</v>
+      </c>
+      <c r="AC48" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD48" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD48" s="36" t="s">
+      <c r="AE48" s="36" t="s">
         <v>562</v>
       </c>
-      <c r="AE48" s="36"/>
       <c r="AF48" s="36"/>
-      <c r="AG48" s="37"/>
-      <c r="AH48" t="s">
+      <c r="AG48" s="36"/>
+      <c r="AH48" s="37"/>
+      <c r="AI48" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="49" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A49" s="33" t="s">
         <v>89</v>
       </c>
@@ -9525,23 +9676,26 @@
       <c r="AA49" s="33">
         <v>2</v>
       </c>
-      <c r="AB49" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC49" s="36" t="s">
+      <c r="AB49" s="33">
+        <v>12</v>
+      </c>
+      <c r="AC49" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD49" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD49" s="36" t="s">
+      <c r="AE49" s="36" t="s">
         <v>554</v>
       </c>
-      <c r="AE49" s="36"/>
       <c r="AF49" s="36"/>
-      <c r="AG49" s="37"/>
-      <c r="AH49" t="s">
+      <c r="AG49" s="36"/>
+      <c r="AH49" s="37"/>
+      <c r="AI49" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="50" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A50" s="33" t="s">
         <v>90</v>
       </c>
@@ -9620,23 +9774,26 @@
       <c r="AA50" s="33">
         <v>2</v>
       </c>
-      <c r="AB50" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC50" s="36" t="s">
+      <c r="AB50" s="33">
+        <v>2</v>
+      </c>
+      <c r="AC50" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD50" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD50" s="36" t="s">
+      <c r="AE50" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE50" s="36"/>
       <c r="AF50" s="36"/>
-      <c r="AG50" s="37"/>
-      <c r="AH50" t="s">
+      <c r="AG50" s="36"/>
+      <c r="AH50" s="37"/>
+      <c r="AI50" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="51" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A51" s="33" t="s">
         <v>88</v>
       </c>
@@ -9715,23 +9872,26 @@
       <c r="AA51" s="33">
         <v>2</v>
       </c>
-      <c r="AB51" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC51" s="36" t="s">
+      <c r="AB51" s="33">
+        <v>15</v>
+      </c>
+      <c r="AC51" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD51" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD51" s="36" t="s">
+      <c r="AE51" s="36" t="s">
         <v>554</v>
       </c>
-      <c r="AE51" s="36"/>
       <c r="AF51" s="36"/>
-      <c r="AG51" s="37"/>
-      <c r="AH51" t="s">
+      <c r="AG51" s="36"/>
+      <c r="AH51" s="37"/>
+      <c r="AI51" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="52" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A52" s="33" t="s">
         <v>85</v>
       </c>
@@ -9810,25 +9970,28 @@
       <c r="AA52" s="33">
         <v>2</v>
       </c>
-      <c r="AB52" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC52" s="36" t="s">
+      <c r="AB52" s="33">
+        <v>24</v>
+      </c>
+      <c r="AC52" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD52" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD52" s="36" t="s">
+      <c r="AE52" s="36" t="s">
         <v>562</v>
       </c>
-      <c r="AE52" s="36"/>
       <c r="AF52" s="36"/>
-      <c r="AG52" s="37" t="s">
+      <c r="AG52" s="36"/>
+      <c r="AH52" s="37" t="s">
         <v>589</v>
       </c>
-      <c r="AH52" t="s">
+      <c r="AI52" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="53" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A53" s="33" t="s">
         <v>375</v>
       </c>
@@ -9897,19 +10060,22 @@
       <c r="AA53" s="33">
         <v>1</v>
       </c>
-      <c r="AB53" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC53" s="36"/>
+      <c r="AB53" s="33">
+        <v>2</v>
+      </c>
+      <c r="AC53" s="34" t="b">
+        <v>1</v>
+      </c>
       <c r="AD53" s="36"/>
       <c r="AE53" s="36"/>
       <c r="AF53" s="36"/>
-      <c r="AG53" s="37"/>
-      <c r="AH53" t="s">
+      <c r="AG53" s="36"/>
+      <c r="AH53" s="37"/>
+      <c r="AI53" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="54" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A54" s="33" t="s">
         <v>86</v>
       </c>
@@ -9988,25 +10154,28 @@
       <c r="AA54" s="33">
         <v>2</v>
       </c>
-      <c r="AB54" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC54" s="36" t="s">
+      <c r="AB54" s="33">
+        <v>8</v>
+      </c>
+      <c r="AC54" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD54" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD54" s="36" t="s">
+      <c r="AE54" s="36" t="s">
         <v>562</v>
       </c>
-      <c r="AE54" s="36"/>
       <c r="AF54" s="36"/>
-      <c r="AG54" s="37" t="s">
+      <c r="AG54" s="36"/>
+      <c r="AH54" s="37" t="s">
         <v>589</v>
       </c>
-      <c r="AH54" t="s">
+      <c r="AI54" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A55" s="33" t="s">
         <v>122</v>
       </c>
@@ -10085,27 +10254,30 @@
       <c r="AA55" s="33">
         <v>2</v>
       </c>
-      <c r="AB55" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC55" s="36" t="s">
+      <c r="AB55" s="33">
+        <v>6</v>
+      </c>
+      <c r="AC55" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD55" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD55" s="36" t="s">
+      <c r="AE55" s="36" t="s">
         <v>562</v>
       </c>
-      <c r="AE55" s="36"/>
-      <c r="AF55" s="36" t="s">
+      <c r="AF55" s="36"/>
+      <c r="AG55" s="36" t="s">
         <v>602</v>
       </c>
-      <c r="AG55" s="37" t="s">
+      <c r="AH55" s="37" t="s">
         <v>604</v>
       </c>
-      <c r="AH55" t="s">
+      <c r="AI55" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="56" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A56" s="33" t="s">
         <v>121</v>
       </c>
@@ -10184,25 +10356,28 @@
       <c r="AA56" s="33">
         <v>2</v>
       </c>
-      <c r="AB56" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC56" s="36" t="s">
+      <c r="AB56" s="33">
+        <v>6</v>
+      </c>
+      <c r="AC56" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD56" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD56" s="36" t="s">
+      <c r="AE56" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE56" s="36" t="s">
+      <c r="AF56" s="36" t="s">
         <v>601</v>
       </c>
-      <c r="AF56" s="36"/>
-      <c r="AG56" s="37"/>
-      <c r="AH56" t="s">
+      <c r="AG56" s="36"/>
+      <c r="AH56" s="37"/>
+      <c r="AI56" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="57" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A57" s="33" t="s">
         <v>101</v>
       </c>
@@ -10281,23 +10456,26 @@
       <c r="AA57" s="33">
         <v>3</v>
       </c>
-      <c r="AB57" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC57" s="36" t="s">
+      <c r="AB57" s="33">
+        <v>9</v>
+      </c>
+      <c r="AC57" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD57" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD57" s="36" t="s">
+      <c r="AE57" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE57" s="36"/>
       <c r="AF57" s="36"/>
-      <c r="AG57" s="37"/>
-      <c r="AH57" t="s">
+      <c r="AG57" s="36"/>
+      <c r="AH57" s="37"/>
+      <c r="AI57" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="58" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A58" s="33" t="s">
         <v>102</v>
       </c>
@@ -10376,25 +10554,28 @@
       <c r="AA58" s="33">
         <v>2</v>
       </c>
-      <c r="AB58" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC58" s="36" t="s">
+      <c r="AB58" s="33">
+        <v>12</v>
+      </c>
+      <c r="AC58" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD58" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD58" s="36" t="s">
+      <c r="AE58" s="36" t="s">
         <v>562</v>
       </c>
-      <c r="AE58" s="36" t="s">
+      <c r="AF58" s="36" t="s">
         <v>599</v>
       </c>
-      <c r="AF58" s="36"/>
-      <c r="AG58" s="37"/>
-      <c r="AH58" t="s">
+      <c r="AG58" s="36"/>
+      <c r="AH58" s="37"/>
+      <c r="AI58" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="59" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A59" s="33" t="s">
         <v>105</v>
       </c>
@@ -10473,25 +10654,28 @@
       <c r="AA59" s="33">
         <v>2</v>
       </c>
-      <c r="AB59" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC59" s="36" t="s">
+      <c r="AB59" s="33">
+        <v>6</v>
+      </c>
+      <c r="AC59" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD59" s="36" t="s">
         <v>549</v>
       </c>
-      <c r="AD59" s="36" t="s">
+      <c r="AE59" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE59" s="36" t="s">
+      <c r="AF59" s="36" t="s">
         <v>599</v>
       </c>
-      <c r="AF59" s="36"/>
-      <c r="AG59" s="37"/>
-      <c r="AH59" t="s">
+      <c r="AG59" s="36"/>
+      <c r="AH59" s="37"/>
+      <c r="AI59" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="60" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A60" s="33" t="s">
         <v>395</v>
       </c>
@@ -10562,19 +10746,22 @@
       <c r="AA60" s="33">
         <v>1</v>
       </c>
-      <c r="AB60" s="34" t="b">
+      <c r="AB60" s="33">
+        <v>1</v>
+      </c>
+      <c r="AC60" s="34" t="b">
         <v>0</v>
       </c>
-      <c r="AC60" s="36"/>
       <c r="AD60" s="36"/>
       <c r="AE60" s="36"/>
       <c r="AF60" s="36"/>
-      <c r="AG60" s="37"/>
-      <c r="AH60" t="s">
+      <c r="AG60" s="36"/>
+      <c r="AH60" s="37"/>
+      <c r="AI60" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="61" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A61" s="33" t="s">
         <v>398</v>
       </c>
@@ -10645,19 +10832,22 @@
       <c r="AA61" s="33">
         <v>1</v>
       </c>
-      <c r="AB61" s="34" t="b">
+      <c r="AB61" s="33">
+        <v>1</v>
+      </c>
+      <c r="AC61" s="34" t="b">
         <v>0</v>
       </c>
-      <c r="AC61" s="36"/>
       <c r="AD61" s="36"/>
       <c r="AE61" s="36"/>
       <c r="AF61" s="36"/>
-      <c r="AG61" s="37"/>
-      <c r="AH61" t="s">
+      <c r="AG61" s="36"/>
+      <c r="AH61" s="37"/>
+      <c r="AI61" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="62" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A62" s="33" t="s">
         <v>402</v>
       </c>
@@ -10728,19 +10918,22 @@
       <c r="AA62" s="33">
         <v>1</v>
       </c>
-      <c r="AB62" s="34" t="b">
+      <c r="AB62" s="33">
+        <v>1</v>
+      </c>
+      <c r="AC62" s="34" t="b">
         <v>0</v>
       </c>
-      <c r="AC62" s="36"/>
       <c r="AD62" s="36"/>
       <c r="AE62" s="36"/>
       <c r="AF62" s="36"/>
-      <c r="AG62" s="37"/>
-      <c r="AH62" t="s">
+      <c r="AG62" s="36"/>
+      <c r="AH62" s="37"/>
+      <c r="AI62" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="63" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A63" s="33" t="s">
         <v>107</v>
       </c>
@@ -10819,25 +11012,28 @@
       <c r="AA63" s="33">
         <v>3</v>
       </c>
-      <c r="AB63" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC63" s="36" t="s">
+      <c r="AB63" s="33">
+        <v>5</v>
+      </c>
+      <c r="AC63" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD63" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD63" s="36" t="s">
+      <c r="AE63" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE63" s="36" t="s">
+      <c r="AF63" s="36" t="s">
         <v>599</v>
       </c>
-      <c r="AF63" s="36"/>
-      <c r="AG63" s="37"/>
-      <c r="AH63" t="s">
+      <c r="AG63" s="36"/>
+      <c r="AH63" s="37"/>
+      <c r="AI63" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="64" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A64" s="33" t="s">
         <v>408</v>
       </c>
@@ -10906,19 +11102,22 @@
       <c r="AA64" s="33">
         <v>1</v>
       </c>
-      <c r="AB64" s="34" t="b">
+      <c r="AB64" s="33">
+        <v>1</v>
+      </c>
+      <c r="AC64" s="34" t="b">
         <v>0</v>
       </c>
-      <c r="AC64" s="36"/>
       <c r="AD64" s="36"/>
       <c r="AE64" s="36"/>
       <c r="AF64" s="36"/>
-      <c r="AG64" s="37"/>
-      <c r="AH64" t="s">
+      <c r="AG64" s="36"/>
+      <c r="AH64" s="37"/>
+      <c r="AI64" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="65" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A65" s="33" t="s">
         <v>106</v>
       </c>
@@ -10997,25 +11196,28 @@
       <c r="AA65" s="33">
         <v>2</v>
       </c>
-      <c r="AB65" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC65" s="36" t="s">
+      <c r="AB65" s="33">
+        <v>6</v>
+      </c>
+      <c r="AC65" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD65" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD65" s="36" t="s">
+      <c r="AE65" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE65" s="36" t="s">
+      <c r="AF65" s="36" t="s">
         <v>599</v>
       </c>
-      <c r="AF65" s="36"/>
-      <c r="AG65" s="37"/>
-      <c r="AH65" t="s">
+      <c r="AG65" s="36"/>
+      <c r="AH65" s="37"/>
+      <c r="AI65" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="66" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A66" s="33" t="s">
         <v>108</v>
       </c>
@@ -11094,23 +11296,26 @@
       <c r="AA66" s="33">
         <v>3</v>
       </c>
-      <c r="AB66" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC66" s="36" t="s">
+      <c r="AB66" s="33">
+        <v>9</v>
+      </c>
+      <c r="AC66" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD66" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD66" s="36" t="s">
+      <c r="AE66" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE66" s="36"/>
       <c r="AF66" s="36"/>
-      <c r="AG66" s="37"/>
-      <c r="AH66" t="s">
+      <c r="AG66" s="36"/>
+      <c r="AH66" s="37"/>
+      <c r="AI66" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="67" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A67" s="33" t="s">
         <v>109</v>
       </c>
@@ -11189,25 +11394,28 @@
       <c r="AA67" s="33">
         <v>2</v>
       </c>
-      <c r="AB67" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC67" s="36" t="s">
+      <c r="AB67" s="33">
+        <v>4</v>
+      </c>
+      <c r="AC67" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD67" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD67" s="36" t="s">
+      <c r="AE67" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE67" s="36" t="s">
+      <c r="AF67" s="36" t="s">
         <v>599</v>
       </c>
-      <c r="AF67" s="36"/>
-      <c r="AG67" s="37"/>
-      <c r="AH67" t="s">
+      <c r="AG67" s="36"/>
+      <c r="AH67" s="37"/>
+      <c r="AI67" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="68" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A68" s="33" t="s">
         <v>110</v>
       </c>
@@ -11286,23 +11494,26 @@
       <c r="AA68" s="33">
         <v>3</v>
       </c>
-      <c r="AB68" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC68" s="36" t="s">
+      <c r="AB68" s="33">
+        <v>3</v>
+      </c>
+      <c r="AC68" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD68" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD68" s="36" t="s">
+      <c r="AE68" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE68" s="36"/>
       <c r="AF68" s="36"/>
-      <c r="AG68" s="37"/>
-      <c r="AH68" t="s">
+      <c r="AG68" s="36"/>
+      <c r="AH68" s="37"/>
+      <c r="AI68" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="69" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A69" s="33" t="s">
         <v>424</v>
       </c>
@@ -11373,19 +11584,22 @@
       <c r="AA69" s="33">
         <v>1</v>
       </c>
-      <c r="AB69" s="34" t="b">
+      <c r="AB69" s="33">
+        <v>3</v>
+      </c>
+      <c r="AC69" s="34" t="b">
         <v>0</v>
       </c>
-      <c r="AC69" s="36"/>
       <c r="AD69" s="36"/>
       <c r="AE69" s="36"/>
       <c r="AF69" s="36"/>
-      <c r="AG69" s="37"/>
-      <c r="AH69" t="s">
+      <c r="AG69" s="36"/>
+      <c r="AH69" s="37"/>
+      <c r="AI69" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="70" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A70" s="33" t="s">
         <v>104</v>
       </c>
@@ -11464,25 +11678,28 @@
       <c r="AA70" s="33">
         <v>2</v>
       </c>
-      <c r="AB70" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC70" s="36" t="s">
+      <c r="AB70" s="33">
+        <v>10</v>
+      </c>
+      <c r="AC70" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD70" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD70" s="36" t="s">
+      <c r="AE70" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE70" s="36" t="s">
+      <c r="AF70" s="36" t="s">
         <v>599</v>
       </c>
-      <c r="AF70" s="36"/>
-      <c r="AG70" s="37"/>
-      <c r="AH70" t="s">
+      <c r="AG70" s="36"/>
+      <c r="AH70" s="37"/>
+      <c r="AI70" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="71" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A71" s="33" t="s">
         <v>103</v>
       </c>
@@ -11561,25 +11778,28 @@
       <c r="AA71" s="33">
         <v>2</v>
       </c>
-      <c r="AB71" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC71" s="36" t="s">
+      <c r="AB71" s="33">
+        <v>6</v>
+      </c>
+      <c r="AC71" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD71" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD71" s="36" t="s">
+      <c r="AE71" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE71" s="36" t="s">
+      <c r="AF71" s="36" t="s">
         <v>599</v>
       </c>
-      <c r="AF71" s="36"/>
-      <c r="AG71" s="37"/>
-      <c r="AH71" t="s">
+      <c r="AG71" s="36"/>
+      <c r="AH71" s="37"/>
+      <c r="AI71" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="72" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A72" s="33" t="s">
         <v>111</v>
       </c>
@@ -11658,25 +11878,28 @@
       <c r="AA72" s="33">
         <v>2</v>
       </c>
-      <c r="AB72" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC72" s="36" t="s">
+      <c r="AB72" s="33">
+        <v>4</v>
+      </c>
+      <c r="AC72" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD72" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD72" s="36" t="s">
+      <c r="AE72" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE72" s="36" t="s">
+      <c r="AF72" s="36" t="s">
         <v>599</v>
       </c>
-      <c r="AF72" s="36"/>
-      <c r="AG72" s="37"/>
-      <c r="AH72" t="s">
+      <c r="AG72" s="36"/>
+      <c r="AH72" s="37"/>
+      <c r="AI72" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="73" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A73" s="33" t="s">
         <v>112</v>
       </c>
@@ -11755,23 +11978,26 @@
       <c r="AA73" s="33">
         <v>2</v>
       </c>
-      <c r="AB73" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC73" s="36" t="s">
+      <c r="AB73" s="33">
+        <v>2</v>
+      </c>
+      <c r="AC73" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD73" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD73" s="36" t="s">
+      <c r="AE73" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE73" s="36"/>
       <c r="AF73" s="36"/>
-      <c r="AG73" s="37"/>
-      <c r="AH73" t="s">
+      <c r="AG73" s="36"/>
+      <c r="AH73" s="37"/>
+      <c r="AI73" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="74" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A74" s="33" t="s">
         <v>113</v>
       </c>
@@ -11850,25 +12076,28 @@
       <c r="AA74" s="33">
         <v>3</v>
       </c>
-      <c r="AB74" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC74" s="36" t="s">
+      <c r="AB74" s="33">
+        <v>6</v>
+      </c>
+      <c r="AC74" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD74" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD74" s="36" t="s">
+      <c r="AE74" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE74" s="36" t="s">
+      <c r="AF74" s="36" t="s">
         <v>599</v>
       </c>
-      <c r="AF74" s="36"/>
-      <c r="AG74" s="37"/>
-      <c r="AH74" t="s">
+      <c r="AG74" s="36"/>
+      <c r="AH74" s="37"/>
+      <c r="AI74" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="75" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A75" s="33" t="s">
         <v>114</v>
       </c>
@@ -11947,23 +12176,26 @@
       <c r="AA75" s="33">
         <v>3</v>
       </c>
-      <c r="AB75" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC75" s="36" t="s">
+      <c r="AB75" s="33">
+        <v>3</v>
+      </c>
+      <c r="AC75" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD75" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD75" s="36" t="s">
+      <c r="AE75" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE75" s="36"/>
       <c r="AF75" s="36"/>
-      <c r="AG75" s="37"/>
-      <c r="AH75" t="s">
+      <c r="AG75" s="36"/>
+      <c r="AH75" s="37"/>
+      <c r="AI75" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="76" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A76" s="33" t="s">
         <v>445</v>
       </c>
@@ -12032,19 +12264,22 @@
       <c r="AA76" s="33">
         <v>2</v>
       </c>
-      <c r="AB76" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC76" s="36"/>
+      <c r="AB76" s="33">
+        <v>2</v>
+      </c>
+      <c r="AC76" s="34" t="b">
+        <v>1</v>
+      </c>
       <c r="AD76" s="36"/>
       <c r="AE76" s="36"/>
       <c r="AF76" s="36"/>
-      <c r="AG76" s="37"/>
-      <c r="AH76" t="s">
+      <c r="AG76" s="36"/>
+      <c r="AH76" s="37"/>
+      <c r="AI76" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="77" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A77" s="33" t="s">
         <v>115</v>
       </c>
@@ -12123,25 +12358,28 @@
       <c r="AA77" s="33">
         <v>3</v>
       </c>
-      <c r="AB77" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC77" s="36" t="s">
+      <c r="AB77" s="33">
+        <v>6</v>
+      </c>
+      <c r="AC77" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD77" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD77" s="36" t="s">
+      <c r="AE77" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE77" s="36" t="s">
+      <c r="AF77" s="36" t="s">
         <v>599</v>
       </c>
-      <c r="AF77" s="36"/>
-      <c r="AG77" s="37"/>
-      <c r="AH77" t="s">
+      <c r="AG77" s="36"/>
+      <c r="AH77" s="37"/>
+      <c r="AI77" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="78" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A78" s="33" t="s">
         <v>116</v>
       </c>
@@ -12220,23 +12458,26 @@
       <c r="AA78" s="33">
         <v>3</v>
       </c>
-      <c r="AB78" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC78" s="36" t="s">
+      <c r="AB78" s="33">
+        <v>4</v>
+      </c>
+      <c r="AC78" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD78" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD78" s="36" t="s">
+      <c r="AE78" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE78" s="36"/>
       <c r="AF78" s="36"/>
-      <c r="AG78" s="37"/>
-      <c r="AH78" t="s">
+      <c r="AG78" s="36"/>
+      <c r="AH78" s="37"/>
+      <c r="AI78" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="79" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A79" s="33" t="s">
         <v>117</v>
       </c>
@@ -12315,23 +12556,26 @@
       <c r="AA79" s="33">
         <v>2</v>
       </c>
-      <c r="AB79" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC79" s="36" t="s">
+      <c r="AB79" s="33">
+        <v>4</v>
+      </c>
+      <c r="AC79" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD79" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD79" s="36" t="s">
+      <c r="AE79" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE79" s="36"/>
       <c r="AF79" s="36"/>
-      <c r="AG79" s="37"/>
-      <c r="AH79" t="s">
+      <c r="AG79" s="36"/>
+      <c r="AH79" s="37"/>
+      <c r="AI79" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="80" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A80" s="33" t="s">
         <v>118</v>
       </c>
@@ -12410,25 +12654,28 @@
       <c r="AA80" s="33">
         <v>2</v>
       </c>
-      <c r="AB80" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC80" s="36" t="s">
+      <c r="AB80" s="33">
+        <v>4</v>
+      </c>
+      <c r="AC80" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD80" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD80" s="36" t="s">
+      <c r="AE80" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE80" s="36" t="s">
+      <c r="AF80" s="36" t="s">
         <v>599</v>
       </c>
-      <c r="AF80" s="36"/>
-      <c r="AG80" s="37"/>
-      <c r="AH80" t="s">
+      <c r="AG80" s="36"/>
+      <c r="AH80" s="37"/>
+      <c r="AI80" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="81" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A81" s="33" t="s">
         <v>119</v>
       </c>
@@ -12507,25 +12754,28 @@
       <c r="AA81" s="33">
         <v>3</v>
       </c>
-      <c r="AB81" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC81" s="36" t="s">
+      <c r="AB81" s="33">
+        <v>3</v>
+      </c>
+      <c r="AC81" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD81" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD81" s="36" t="s">
+      <c r="AE81" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE81" s="36" t="s">
+      <c r="AF81" s="36" t="s">
         <v>599</v>
       </c>
-      <c r="AF81" s="36"/>
-      <c r="AG81" s="37"/>
-      <c r="AH81" t="s">
+      <c r="AG81" s="36"/>
+      <c r="AH81" s="37"/>
+      <c r="AI81" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="82" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A82" s="33" t="s">
         <v>462</v>
       </c>
@@ -12594,19 +12844,22 @@
       <c r="AA82" s="33">
         <v>6</v>
       </c>
-      <c r="AB82" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC82" s="36"/>
+      <c r="AB82" s="33">
+        <v>6</v>
+      </c>
+      <c r="AC82" s="34" t="b">
+        <v>1</v>
+      </c>
       <c r="AD82" s="36"/>
       <c r="AE82" s="36"/>
       <c r="AF82" s="36"/>
-      <c r="AG82" s="37"/>
-      <c r="AH82" t="s">
+      <c r="AG82" s="36"/>
+      <c r="AH82" s="37"/>
+      <c r="AI82" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="83" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A83" s="33" t="s">
         <v>123</v>
       </c>
@@ -12685,23 +12938,26 @@
       <c r="AA83" s="33">
         <v>1</v>
       </c>
-      <c r="AB83" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC83" s="36" t="s">
+      <c r="AB83" s="33">
+        <v>6</v>
+      </c>
+      <c r="AC83" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD83" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD83" s="36" t="s">
+      <c r="AE83" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE83" s="36"/>
       <c r="AF83" s="36"/>
-      <c r="AG83" s="37"/>
-      <c r="AH83" t="s">
+      <c r="AG83" s="36"/>
+      <c r="AH83" s="37"/>
+      <c r="AI83" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="84" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A84" s="33" t="s">
         <v>124</v>
       </c>
@@ -12780,25 +13036,28 @@
       <c r="AA84" s="33">
         <v>1</v>
       </c>
-      <c r="AB84" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC84" s="36" t="s">
+      <c r="AB84" s="33">
+        <v>6</v>
+      </c>
+      <c r="AC84" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD84" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD84" s="36" t="s">
+      <c r="AE84" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE84" s="36"/>
       <c r="AF84" s="36"/>
-      <c r="AG84" s="37" t="s">
+      <c r="AG84" s="36"/>
+      <c r="AH84" s="37" t="s">
         <v>605</v>
       </c>
-      <c r="AH84" t="s">
+      <c r="AI84" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="85" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A85" s="33" t="s">
         <v>125</v>
       </c>
@@ -12877,27 +13136,30 @@
       <c r="AA85" s="33">
         <v>2</v>
       </c>
-      <c r="AB85" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC85" s="36" t="s">
+      <c r="AB85" s="33">
+        <v>4</v>
+      </c>
+      <c r="AC85" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD85" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD85" s="36" t="s">
+      <c r="AE85" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE85" s="36" t="s">
+      <c r="AF85" s="36" t="s">
         <v>606</v>
       </c>
-      <c r="AF85" s="36" t="s">
+      <c r="AG85" s="36" t="s">
         <v>602</v>
       </c>
-      <c r="AG85" s="37"/>
-      <c r="AH85" t="s">
+      <c r="AH85" s="37"/>
+      <c r="AI85" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="86" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A86" s="33" t="s">
         <v>475</v>
       </c>
@@ -12966,19 +13228,22 @@
       <c r="AA86" s="33">
         <v>2</v>
       </c>
-      <c r="AB86" s="34" t="b">
+      <c r="AB86" s="33">
+        <v>4</v>
+      </c>
+      <c r="AC86" s="34" t="b">
         <v>0</v>
       </c>
-      <c r="AC86" s="36"/>
       <c r="AD86" s="36"/>
       <c r="AE86" s="36"/>
       <c r="AF86" s="36"/>
-      <c r="AG86" s="37"/>
-      <c r="AH86" t="s">
+      <c r="AG86" s="36"/>
+      <c r="AH86" s="37"/>
+      <c r="AI86" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="87" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A87" s="33" t="s">
         <v>126</v>
       </c>
@@ -13057,23 +13322,26 @@
       <c r="AA87" s="33">
         <v>2</v>
       </c>
-      <c r="AB87" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC87" s="36" t="s">
+      <c r="AB87" s="33">
+        <v>13</v>
+      </c>
+      <c r="AC87" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD87" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD87" s="36" t="s">
+      <c r="AE87" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE87" s="36"/>
       <c r="AF87" s="36"/>
-      <c r="AG87" s="37"/>
-      <c r="AH87" t="s">
+      <c r="AG87" s="36"/>
+      <c r="AH87" s="37"/>
+      <c r="AI87" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="88" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A88" s="33" t="s">
         <v>127</v>
       </c>
@@ -13152,23 +13420,26 @@
       <c r="AA88" s="33">
         <v>2</v>
       </c>
-      <c r="AB88" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC88" s="36" t="s">
+      <c r="AB88" s="33">
+        <v>8</v>
+      </c>
+      <c r="AC88" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD88" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD88" s="36" t="s">
+      <c r="AE88" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE88" s="36"/>
       <c r="AF88" s="36"/>
-      <c r="AG88" s="37"/>
-      <c r="AH88" t="s">
+      <c r="AG88" s="36"/>
+      <c r="AH88" s="37"/>
+      <c r="AI88" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="89" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A89" s="33" t="s">
         <v>128</v>
       </c>
@@ -13247,25 +13518,28 @@
       <c r="AA89" s="33">
         <v>1</v>
       </c>
-      <c r="AB89" s="34" t="b">
+      <c r="AB89" s="33">
+        <v>4</v>
+      </c>
+      <c r="AC89" s="34" t="b">
         <v>0</v>
       </c>
-      <c r="AC89" s="36" t="s">
+      <c r="AD89" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD89" s="36" t="s">
+      <c r="AE89" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE89" s="36"/>
-      <c r="AF89" s="36" t="s">
+      <c r="AF89" s="36"/>
+      <c r="AG89" s="36" t="s">
         <v>608</v>
       </c>
-      <c r="AG89" s="37"/>
-      <c r="AH89" t="s">
+      <c r="AH89" s="37"/>
+      <c r="AI89" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="90" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A90" s="33" t="s">
         <v>74</v>
       </c>
@@ -13344,25 +13618,28 @@
       <c r="AA90" s="33">
         <v>2</v>
       </c>
-      <c r="AB90" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC90" s="36" t="s">
+      <c r="AB90" s="33">
+        <v>2</v>
+      </c>
+      <c r="AC90" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD90" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD90" s="36" t="s">
+      <c r="AE90" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE90" s="36"/>
-      <c r="AF90" s="36" t="s">
+      <c r="AF90" s="36"/>
+      <c r="AG90" s="36" t="s">
         <v>577</v>
       </c>
-      <c r="AG90" s="37"/>
-      <c r="AH90" t="s">
+      <c r="AH90" s="37"/>
+      <c r="AI90" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="91" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A91" s="33" t="s">
         <v>83</v>
       </c>
@@ -13441,25 +13718,28 @@
       <c r="AA91" s="33">
         <v>2</v>
       </c>
-      <c r="AB91" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC91" s="36" t="s">
+      <c r="AB91" s="33">
+        <v>7</v>
+      </c>
+      <c r="AC91" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD91" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD91" s="36" t="s">
+      <c r="AE91" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE91" s="36"/>
-      <c r="AF91" s="36" t="s">
+      <c r="AF91" s="36"/>
+      <c r="AG91" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="AG91" s="37"/>
-      <c r="AH91" s="36" t="s">
+      <c r="AH91" s="37"/>
+      <c r="AI91" s="36" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="92" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A92" s="33" t="s">
         <v>75</v>
       </c>
@@ -13538,25 +13818,28 @@
       <c r="AA92" s="33">
         <v>1</v>
       </c>
-      <c r="AB92" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC92" s="36" t="s">
+      <c r="AB92" s="33">
+        <v>4</v>
+      </c>
+      <c r="AC92" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD92" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD92" s="36" t="s">
+      <c r="AE92" s="36" t="s">
         <v>562</v>
       </c>
-      <c r="AE92" s="36"/>
-      <c r="AF92" s="36" t="s">
+      <c r="AF92" s="36"/>
+      <c r="AG92" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="AG92" s="37"/>
-      <c r="AH92" t="s">
+      <c r="AH92" s="37"/>
+      <c r="AI92" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="93" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A93" s="33" t="s">
         <v>76</v>
       </c>
@@ -13635,25 +13918,28 @@
       <c r="AA93" s="33">
         <v>1</v>
       </c>
-      <c r="AB93" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC93" s="36" t="s">
+      <c r="AB93" s="33">
+        <v>5</v>
+      </c>
+      <c r="AC93" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD93" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="AD93" s="36" t="s">
+      <c r="AE93" s="36" t="s">
         <v>562</v>
       </c>
-      <c r="AE93" s="36"/>
-      <c r="AF93" s="36" t="s">
+      <c r="AF93" s="36"/>
+      <c r="AG93" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="AG93" s="37"/>
-      <c r="AH93" t="s">
+      <c r="AH93" s="37"/>
+      <c r="AI93" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="94" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A94" s="33" t="s">
         <v>77</v>
       </c>
@@ -13732,25 +14018,28 @@
       <c r="AA94" s="33">
         <v>2</v>
       </c>
-      <c r="AB94" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC94" s="36" t="s">
+      <c r="AB94" s="33">
+        <v>4</v>
+      </c>
+      <c r="AC94" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD94" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD94" s="36" t="s">
+      <c r="AE94" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE94" s="36"/>
-      <c r="AF94" s="36" t="s">
+      <c r="AF94" s="36"/>
+      <c r="AG94" s="36" t="s">
         <v>577</v>
       </c>
-      <c r="AG94" s="37"/>
-      <c r="AH94" t="s">
+      <c r="AH94" s="37"/>
+      <c r="AI94" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="95" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A95" s="33" t="s">
         <v>499</v>
       </c>
@@ -13821,19 +14110,22 @@
       <c r="AA95" s="33">
         <v>2</v>
       </c>
-      <c r="AB95" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC95" s="36"/>
+      <c r="AB95" s="33">
+        <v>4</v>
+      </c>
+      <c r="AC95" s="34" t="b">
+        <v>1</v>
+      </c>
       <c r="AD95" s="36"/>
       <c r="AE95" s="36"/>
       <c r="AF95" s="36"/>
-      <c r="AG95" s="37"/>
-      <c r="AH95" t="s">
+      <c r="AG95" s="36"/>
+      <c r="AH95" s="37"/>
+      <c r="AI95" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="96" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A96" s="33" t="s">
         <v>78</v>
       </c>
@@ -13912,25 +14204,28 @@
       <c r="AA96" s="33">
         <v>2</v>
       </c>
-      <c r="AB96" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC96" s="36" t="s">
+      <c r="AB96" s="33">
+        <v>4</v>
+      </c>
+      <c r="AC96" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD96" s="36" t="s">
         <v>549</v>
       </c>
-      <c r="AD96" s="36" t="s">
+      <c r="AE96" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE96" s="36"/>
-      <c r="AF96" s="36" t="s">
+      <c r="AF96" s="36"/>
+      <c r="AG96" s="36" t="s">
         <v>577</v>
       </c>
-      <c r="AG96" s="37"/>
-      <c r="AH96" t="s">
+      <c r="AH96" s="37"/>
+      <c r="AI96" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="97" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A97" s="33" t="s">
         <v>79</v>
       </c>
@@ -14009,25 +14304,28 @@
       <c r="AA97" s="33">
         <v>2</v>
       </c>
-      <c r="AB97" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC97" s="36" t="s">
+      <c r="AB97" s="33">
+        <v>6</v>
+      </c>
+      <c r="AC97" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD97" s="36" t="s">
         <v>549</v>
       </c>
-      <c r="AD97" s="36" t="s">
+      <c r="AE97" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE97" s="36"/>
-      <c r="AF97" s="36" t="s">
+      <c r="AF97" s="36"/>
+      <c r="AG97" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="AG97" s="37"/>
-      <c r="AH97" t="s">
+      <c r="AH97" s="37"/>
+      <c r="AI97" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="98" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A98" s="33" t="s">
         <v>80</v>
       </c>
@@ -14106,25 +14404,28 @@
       <c r="AA98" s="33">
         <v>2</v>
       </c>
-      <c r="AB98" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC98" s="36" t="s">
+      <c r="AB98" s="33">
+        <v>2</v>
+      </c>
+      <c r="AC98" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD98" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD98" s="36" t="s">
+      <c r="AE98" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE98" s="36"/>
-      <c r="AF98" s="36" t="s">
+      <c r="AF98" s="36"/>
+      <c r="AG98" s="36" t="s">
         <v>577</v>
       </c>
-      <c r="AG98" s="37"/>
-      <c r="AH98" t="s">
+      <c r="AH98" s="37"/>
+      <c r="AI98" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="99" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A99" s="33" t="s">
         <v>81</v>
       </c>
@@ -14203,25 +14504,28 @@
       <c r="AA99" s="33">
         <v>2</v>
       </c>
-      <c r="AB99" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC99" s="36" t="s">
+      <c r="AB99" s="33">
+        <v>4</v>
+      </c>
+      <c r="AC99" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD99" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD99" s="36" t="s">
+      <c r="AE99" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE99" s="36"/>
-      <c r="AF99" s="36" t="s">
+      <c r="AF99" s="36"/>
+      <c r="AG99" s="36" t="s">
         <v>577</v>
       </c>
-      <c r="AG99" s="37"/>
-      <c r="AH99" t="s">
+      <c r="AH99" s="37"/>
+      <c r="AI99" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="100" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A100" s="33" t="s">
         <v>82</v>
       </c>
@@ -14300,27 +14604,30 @@
       <c r="AA100" s="33">
         <v>2</v>
       </c>
-      <c r="AB100" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC100" s="36" t="s">
+      <c r="AB100" s="33">
+        <v>6</v>
+      </c>
+      <c r="AC100" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD100" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD100" s="36" t="s">
+      <c r="AE100" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE100" s="36"/>
-      <c r="AF100" s="36" t="s">
+      <c r="AF100" s="36"/>
+      <c r="AG100" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="AG100" s="37" t="s">
+      <c r="AH100" s="37" t="s">
         <v>628</v>
       </c>
-      <c r="AH100" t="s">
+      <c r="AI100" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="101" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A101" s="33" t="s">
         <v>84</v>
       </c>
@@ -14399,23 +14706,26 @@
       <c r="AA101" s="33">
         <v>2</v>
       </c>
-      <c r="AB101" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC101" s="36" t="s">
+      <c r="AB101" s="33">
+        <v>8</v>
+      </c>
+      <c r="AC101" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD101" s="36" t="s">
         <v>550</v>
       </c>
-      <c r="AD101" s="36" t="s">
+      <c r="AE101" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="AE101" s="36"/>
-      <c r="AF101" s="36" t="s">
+      <c r="AF101" s="36"/>
+      <c r="AG101" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="AG101" s="37" t="s">
+      <c r="AH101" s="37" t="s">
         <v>628</v>
       </c>
-      <c r="AH101" t="s">
+      <c r="AI101" t="s">
         <v>519</v>
       </c>
     </row>
@@ -14430,7 +14740,7 @@
   <dimension ref="A1:P44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>